<commit_message>
- Added parameter -InsertLicense for setting the NSX license in vCenter, which is required from NSX 6.2.3 and on before you can prepare your hosts
</commit_message>
<xml_diff>
--- a/install-nsx-info-example.xlsx
+++ b/install-nsx-info-example.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="702"/>
   </bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Distributed Logical Routers" sheetId="8" r:id="rId6"/>
     <sheet name="Options" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="A5" authorId="0" shapeId="0">
@@ -40,7 +40,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -112,7 +112,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -136,7 +136,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -160,7 +160,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -184,7 +184,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -205,7 +205,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="H1" authorId="0" shapeId="0">
@@ -218,7 +218,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -263,7 +263,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Auteur</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0">
@@ -276,7 +276,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Auteur:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="115">
   <si>
     <t>NSX Manager information</t>
   </si>
@@ -679,11 +679,17 @@
   <si>
     <t>239.0.200.254</t>
   </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>xxx-xxx-xxx-xxx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -764,7 +770,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1079,7 +1085,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,6 +1195,9 @@
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1211,6 +1220,9 @@
       </c>
       <c r="G7" t="s">
         <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>